<commit_message>
Updated Nithin as Director of Fundraising and accepted majors in FAQs
</commit_message>
<xml_diff>
--- a/src/data/summerfall23/directors_summerfall23.xlsx
+++ b/src/data/summerfall23/directors_summerfall23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\kcow\code\dspuci-website-gatsby\src\data\summerfall23\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abigailbareiss/dspuci-website-gatsby/src/data/summerfall23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCE7200-EDE6-4D46-9646-FD9A27F1A84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8BE64B-6CAC-DC43-B51D-5E6FABB5664C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
+    <workbookView xWindow="14400" yWindow="760" windowWidth="14400" windowHeight="15600" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>Brennan Kim</t>
   </si>
   <si>
-    <t>Winnie Qi</t>
-  </si>
-  <si>
     <t>Juliana Lee</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Allison Chu</t>
+  </si>
+  <si>
+    <t>Nithin Senthil</t>
   </si>
 </sst>
 </file>
@@ -461,12 +461,12 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.75" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -475,16 +475,16 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -493,7 +493,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -502,45 +502,45 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>

</xml_diff>